<commit_message>
R: add Bibliometrix & Boxplot
</commit_message>
<xml_diff>
--- a/R/assets/Data Total.xlsx
+++ b/R/assets/Data Total.xlsx
@@ -1527,7 +1527,7 @@
         <v>10.39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>10.33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>18.15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>18.32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>20.21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>22.76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>20.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>12.46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>13.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>11.58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>16.32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
       <c r="A24" s="5" t="s">
         <v>33</v>
       </c>

</xml_diff>